<commit_message>
Data as on 9-1-21-Morning
</commit_message>
<xml_diff>
--- a/0. Files/1. Water Quality/5. Data/2. Calibration/TDS-Data.xlsx
+++ b/0. Files/1. Water Quality/5. Data/2. Calibration/TDS-Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Desktop\Files\1. Projects\1. Water Quality\5. Data\2. Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Jupyter Notebooks\Projects\WaterDataAnalysis\0. Files\1. Water Quality\5. Data\2. Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CD0987-6F71-4F72-9D47-9C825B0CC80A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41DAC68-5CA8-4ED3-8413-8470A8BC4E25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:N364"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1197,7 @@
         <v>91</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I12" si="0">(G3+H3)/2</f>
+        <f t="shared" ref="I3:I11" si="0">(G3+H3)/2</f>
         <v>91</v>
       </c>
       <c r="J3" s="2"/>
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="1"/>
+        <f>(126*100*J7+332*100*K7+70*L7*100)/(100*J7+100*K7+L7*100+M7*100)</f>
         <v>70</v>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="1"/>
+        <f>(126*100*J9+324*100*K9+70*L9*100)/(100*J9+100*K9+L9*100+M9*100)</f>
         <v>70</v>
       </c>
     </row>
@@ -1503,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="1"/>
+        <f>(126*100*J10+324*100*K10+70*L10*100)/(100*J10+100*K10+L10*100+M10*100)</f>
         <v>70</v>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
         <v>82</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" ref="I14:I23" si="2">(H14+G14)/2</f>
+        <f t="shared" ref="I14:I22" si="2">(H14+G14)/2</f>
         <v>81</v>
       </c>
       <c r="J14" s="3"/>
@@ -2522,15 +2522,23 @@
       <c r="B35" s="5">
         <v>50</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="5">
+        <v>7.8974000000000003E-2</v>
+      </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="F35" s="5">
+        <v>22</v>
+      </c>
+      <c r="G35" s="5">
+        <v>56</v>
+      </c>
+      <c r="H35" s="5">
+        <v>46</v>
+      </c>
       <c r="I35" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2552,15 +2560,23 @@
       <c r="B36" s="5">
         <v>48</v>
       </c>
-      <c r="C36" s="5"/>
+      <c r="C36" s="5">
+        <v>7.4138999999999997E-2</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="F36" s="5">
+        <v>21</v>
+      </c>
+      <c r="G36" s="5">
+        <v>49</v>
+      </c>
+      <c r="H36" s="5">
+        <v>45</v>
+      </c>
       <c r="I36" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -2582,15 +2598,23 @@
       <c r="B37" s="5">
         <v>45</v>
       </c>
-      <c r="C37" s="5"/>
+      <c r="C37" s="5">
+        <v>6.4468999999999999E-2</v>
+      </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="F37" s="5">
+        <v>19</v>
+      </c>
+      <c r="G37" s="5">
+        <v>46</v>
+      </c>
+      <c r="H37" s="5">
+        <v>45</v>
+      </c>
       <c r="I37" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>45.5</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -2612,15 +2636,23 @@
       <c r="B38" s="5">
         <v>42</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="5">
+        <v>5.6410000000000002E-2</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="F38" s="5">
+        <v>18</v>
+      </c>
+      <c r="G38" s="5">
+        <v>45</v>
+      </c>
+      <c r="H38" s="5">
+        <v>47</v>
+      </c>
       <c r="I38" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
@@ -2642,15 +2674,23 @@
       <c r="B39" s="5">
         <v>40</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="5">
+        <v>5.1575000000000003E-2</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+      <c r="F39" s="5">
+        <v>17</v>
+      </c>
+      <c r="G39" s="5">
+        <v>45</v>
+      </c>
+      <c r="H39" s="5">
+        <v>45</v>
+      </c>
       <c r="I39" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
@@ -2672,15 +2712,23 @@
       <c r="B40" s="5">
         <v>38</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="5">
+        <v>4.7545999999999998E-2</v>
+      </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+      <c r="F40" s="5">
+        <v>16</v>
+      </c>
+      <c r="G40" s="5">
+        <v>47</v>
+      </c>
+      <c r="H40" s="5">
+        <v>45</v>
+      </c>
       <c r="I40" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -2702,15 +2750,23 @@
       <c r="B41" s="5">
         <v>35</v>
       </c>
-      <c r="C41" s="5"/>
+      <c r="C41" s="5">
+        <v>3.9487000000000001E-2</v>
+      </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="F41" s="5">
+        <v>14</v>
+      </c>
+      <c r="G41" s="5">
+        <v>45</v>
+      </c>
+      <c r="H41" s="5">
+        <v>46</v>
+      </c>
       <c r="I41" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>45.5</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
@@ -2732,15 +2788,23 @@
       <c r="B42" s="5">
         <v>32</v>
       </c>
-      <c r="C42" s="5"/>
+      <c r="C42" s="5">
+        <v>3.304E-2</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+      <c r="F42" s="5">
+        <v>12</v>
+      </c>
+      <c r="G42" s="5">
+        <v>45</v>
+      </c>
+      <c r="H42" s="5">
+        <v>45</v>
+      </c>
       <c r="I42" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
@@ -2762,15 +2826,23 @@
       <c r="B43" s="5">
         <v>30</v>
       </c>
-      <c r="C43" s="5"/>
+      <c r="C43" s="5">
+        <v>2.6592999999999999E-2</v>
+      </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="F43" s="5">
+        <v>10</v>
+      </c>
+      <c r="G43" s="5">
+        <v>44</v>
+      </c>
+      <c r="H43" s="5">
+        <v>39</v>
+      </c>
       <c r="I43" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>41.5</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
@@ -2792,15 +2864,23 @@
       <c r="B44" s="5">
         <v>28</v>
       </c>
-      <c r="C44" s="5"/>
+      <c r="C44" s="5">
+        <v>2.2564000000000001E-2</v>
+      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+      <c r="F44" s="5">
+        <v>9</v>
+      </c>
+      <c r="G44" s="5">
+        <v>45</v>
+      </c>
+      <c r="H44" s="5">
+        <v>42</v>
+      </c>
       <c r="I44" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>43.5</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
@@ -2822,15 +2902,23 @@
       <c r="B45" s="5">
         <v>25</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5">
+        <v>1.5311E-2</v>
+      </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+      <c r="F45" s="5">
+        <v>7</v>
+      </c>
+      <c r="G45" s="5">
+        <v>40</v>
+      </c>
+      <c r="H45" s="5">
+        <v>44</v>
+      </c>
       <c r="I45" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
@@ -2852,15 +2940,23 @@
       <c r="B46" s="6">
         <v>50</v>
       </c>
-      <c r="C46" s="6"/>
+      <c r="C46" s="6">
+        <v>5.8021999999999997E-2</v>
+      </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
+      <c r="F46" s="6">
+        <v>16</v>
+      </c>
+      <c r="G46" s="6">
+        <v>40</v>
+      </c>
+      <c r="H46" s="6">
+        <v>46</v>
+      </c>
       <c r="I46" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -2882,15 +2978,23 @@
       <c r="B47" s="6">
         <v>48</v>
       </c>
-      <c r="C47" s="6"/>
+      <c r="C47" s="6">
+        <v>5.3186999999999998E-2</v>
+      </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="F47" s="6">
+        <v>15</v>
+      </c>
+      <c r="G47" s="6">
+        <v>43</v>
+      </c>
+      <c r="H47" s="6">
+        <v>39</v>
+      </c>
       <c r="I47" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -2912,15 +3016,23 @@
       <c r="B48" s="6">
         <v>45</v>
       </c>
-      <c r="C48" s="6"/>
+      <c r="C48" s="6">
+        <v>4.7545999999999998E-2</v>
+      </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
+      <c r="F48" s="6">
+        <v>14</v>
+      </c>
+      <c r="G48" s="6">
+        <v>45</v>
+      </c>
+      <c r="H48" s="6">
+        <v>40</v>
+      </c>
       <c r="I48" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>42.5</v>
       </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -2942,15 +3054,23 @@
       <c r="B49" s="6">
         <v>42</v>
       </c>
-      <c r="C49" s="6"/>
+      <c r="C49" s="6">
+        <v>3.8681E-2</v>
+      </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="F49" s="6">
+        <v>12</v>
+      </c>
+      <c r="G49" s="6">
+        <v>44</v>
+      </c>
+      <c r="H49" s="6">
+        <v>45</v>
+      </c>
       <c r="I49" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>44.5</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -2972,15 +3092,23 @@
       <c r="B50" s="6">
         <v>40</v>
       </c>
-      <c r="C50" s="6"/>
+      <c r="C50" s="6">
+        <v>3.7874999999999999E-2</v>
+      </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
+      <c r="F50" s="6">
+        <v>12</v>
+      </c>
+      <c r="G50" s="6">
+        <v>40</v>
+      </c>
+      <c r="H50" s="6">
+        <v>44</v>
+      </c>
       <c r="I50" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -3002,15 +3130,23 @@
       <c r="B51" s="6">
         <v>38</v>
       </c>
-      <c r="C51" s="6"/>
+      <c r="C51" s="6">
+        <v>3.3846000000000001E-2</v>
+      </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
+      <c r="F51" s="6">
+        <v>11</v>
+      </c>
+      <c r="G51" s="6">
+        <v>43</v>
+      </c>
+      <c r="H51" s="6">
+        <v>40</v>
+      </c>
       <c r="I51" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>41.5</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -3032,15 +3168,23 @@
       <c r="B52" s="6">
         <v>35</v>
       </c>
-      <c r="C52" s="6"/>
+      <c r="C52" s="6">
+        <v>2.4982000000000001E-2</v>
+      </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
+      <c r="F52" s="6">
+        <v>9</v>
+      </c>
+      <c r="G52" s="6">
+        <v>40</v>
+      </c>
+      <c r="H52" s="6">
+        <v>41</v>
+      </c>
       <c r="I52" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40.5</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -3062,15 +3206,23 @@
       <c r="B53" s="6">
         <v>32</v>
       </c>
-      <c r="C53" s="6"/>
+      <c r="C53" s="6">
+        <v>1.8534999999999999E-2</v>
+      </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
+      <c r="F53" s="6">
+        <v>7</v>
+      </c>
+      <c r="G53" s="6">
+        <v>41</v>
+      </c>
+      <c r="H53" s="6">
+        <v>41</v>
+      </c>
       <c r="I53" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -3092,15 +3244,23 @@
       <c r="B54" s="6">
         <v>30</v>
       </c>
-      <c r="C54" s="6"/>
+      <c r="C54" s="6">
+        <v>1.37E-2</v>
+      </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
+      <c r="F54" s="6">
+        <v>5</v>
+      </c>
+      <c r="G54" s="6">
+        <v>38</v>
+      </c>
+      <c r="H54" s="6">
+        <v>40</v>
+      </c>
       <c r="I54" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -3122,15 +3282,23 @@
       <c r="B55" s="6">
         <v>28</v>
       </c>
-      <c r="C55" s="6"/>
+      <c r="C55" s="6">
+        <v>1.1282E-2</v>
+      </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
+      <c r="F55" s="6">
+        <v>5</v>
+      </c>
+      <c r="G55" s="6">
+        <v>38</v>
+      </c>
+      <c r="H55" s="6">
+        <v>40</v>
+      </c>
       <c r="I55" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -3152,15 +3320,23 @@
       <c r="B56" s="6">
         <v>25</v>
       </c>
-      <c r="C56" s="6"/>
+      <c r="C56" s="6">
+        <v>0</v>
+      </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
+      <c r="F56" s="6">
+        <v>0</v>
+      </c>
+      <c r="G56" s="6">
+        <v>35</v>
+      </c>
+      <c r="H56" s="6">
+        <v>39</v>
+      </c>
       <c r="I56" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -3182,15 +3358,23 @@
       <c r="B57" s="7">
         <v>50</v>
       </c>
-      <c r="C57" s="7"/>
+      <c r="C57" s="7">
+        <v>5.1575000000000003E-2</v>
+      </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
+      <c r="F57" s="7">
+        <v>15</v>
+      </c>
+      <c r="G57" s="7">
+        <v>39</v>
+      </c>
+      <c r="H57" s="7">
+        <v>46</v>
+      </c>
       <c r="I57" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>42.5</v>
       </c>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
@@ -3212,15 +3396,23 @@
       <c r="B58" s="7">
         <v>48</v>
       </c>
-      <c r="C58" s="7"/>
+      <c r="C58" s="7">
+        <v>4.5934000000000003E-2</v>
+      </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
+      <c r="F58" s="7">
+        <v>13</v>
+      </c>
+      <c r="G58" s="7">
+        <v>43</v>
+      </c>
+      <c r="H58" s="7">
+        <v>39</v>
+      </c>
       <c r="I58" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
@@ -3242,15 +3434,23 @@
       <c r="B59" s="7">
         <v>45</v>
       </c>
-      <c r="C59" s="7"/>
+      <c r="C59" s="7">
+        <v>3.8681E-2</v>
+      </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
+      <c r="F59" s="7">
+        <v>12</v>
+      </c>
+      <c r="G59" s="7">
+        <v>39</v>
+      </c>
+      <c r="H59" s="7">
+        <v>43</v>
+      </c>
       <c r="I59" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
@@ -3272,15 +3472,23 @@
       <c r="B60" s="7">
         <v>42</v>
       </c>
-      <c r="C60" s="7"/>
+      <c r="C60" s="7">
+        <v>3.304E-2</v>
+      </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
+      <c r="F60" s="7">
+        <v>10</v>
+      </c>
+      <c r="G60" s="7">
+        <v>37</v>
+      </c>
+      <c r="H60" s="7">
+        <v>43</v>
+      </c>
       <c r="I60" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
@@ -3302,15 +3510,23 @@
       <c r="B61" s="7">
         <v>40</v>
       </c>
-      <c r="C61" s="7"/>
+      <c r="C61" s="7">
+        <v>2.8205000000000001E-2</v>
+      </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
+      <c r="F61" s="7">
+        <v>9</v>
+      </c>
+      <c r="G61" s="7">
+        <v>38</v>
+      </c>
+      <c r="H61" s="7">
+        <v>41</v>
+      </c>
       <c r="I61" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>39.5</v>
       </c>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
@@ -3332,15 +3548,23 @@
       <c r="B62" s="7">
         <v>38</v>
       </c>
-      <c r="C62" s="7"/>
+      <c r="C62" s="7">
+        <v>2.4982000000000001E-2</v>
+      </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
+      <c r="F62" s="7">
+        <v>8</v>
+      </c>
+      <c r="G62" s="7">
+        <v>38</v>
+      </c>
+      <c r="H62" s="7">
+        <v>39</v>
+      </c>
       <c r="I62" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>38.5</v>
       </c>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
@@ -3362,15 +3586,23 @@
       <c r="B63" s="7">
         <v>35</v>
       </c>
-      <c r="C63" s="7"/>
+      <c r="C63" s="7">
+        <v>1.6923000000000001E-2</v>
+      </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
+      <c r="F63" s="7">
+        <v>6</v>
+      </c>
+      <c r="G63" s="7">
+        <v>38</v>
+      </c>
+      <c r="H63" s="7">
+        <v>39</v>
+      </c>
       <c r="I63" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>38.5</v>
       </c>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
@@ -3392,15 +3624,23 @@
       <c r="B64" s="7">
         <v>32</v>
       </c>
-      <c r="C64" s="7"/>
+      <c r="C64" s="7">
+        <v>1.2893999999999999E-2</v>
+      </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
+      <c r="F64" s="7">
+        <v>5</v>
+      </c>
+      <c r="G64" s="7">
+        <v>38</v>
+      </c>
+      <c r="H64" s="7">
+        <v>38</v>
+      </c>
       <c r="I64" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
@@ -3422,15 +3662,23 @@
       <c r="B65" s="7">
         <v>30</v>
       </c>
-      <c r="C65" s="7"/>
+      <c r="C65" s="7">
+        <v>5.6410000000000002E-3</v>
+      </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
+      <c r="F65" s="7">
+        <v>2</v>
+      </c>
+      <c r="G65" s="7">
+        <v>37</v>
+      </c>
+      <c r="H65" s="7">
+        <v>38</v>
+      </c>
       <c r="I65" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
@@ -3452,15 +3700,23 @@
       <c r="B66" s="7">
         <v>28</v>
       </c>
-      <c r="C66" s="7"/>
+      <c r="C66" s="7">
+        <v>1.6119999999999999E-3</v>
+      </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
+      <c r="F66" s="7">
+        <v>1</v>
+      </c>
+      <c r="G66" s="7">
+        <v>35</v>
+      </c>
+      <c r="H66" s="7">
+        <v>38</v>
+      </c>
       <c r="I66" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>36.5</v>
       </c>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
@@ -3482,15 +3738,27 @@
       <c r="B67" s="7">
         <v>25</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
+      <c r="C67" s="7">
+        <v>0</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0</v>
+      </c>
+      <c r="G67" s="7">
+        <v>31</v>
+      </c>
+      <c r="H67" s="7">
+        <v>36</v>
+      </c>
       <c r="I67" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>33.5</v>
       </c>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
@@ -3512,15 +3780,23 @@
       <c r="B68" s="8">
         <v>50</v>
       </c>
-      <c r="C68" s="8"/>
+      <c r="C68" s="8">
+        <v>2.9817E-2</v>
+      </c>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
+      <c r="F68" s="8">
+        <v>8</v>
+      </c>
+      <c r="G68" s="8">
+        <v>42</v>
+      </c>
+      <c r="H68" s="8">
+        <v>33</v>
+      </c>
       <c r="I68" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="8"/>
@@ -3542,15 +3818,23 @@
       <c r="B69" s="8">
         <v>48</v>
       </c>
-      <c r="C69" s="8"/>
+      <c r="C69" s="8">
+        <v>2.4176E-2</v>
+      </c>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
+      <c r="F69" s="8">
+        <v>7</v>
+      </c>
+      <c r="G69" s="8">
+        <v>33</v>
+      </c>
+      <c r="H69" s="8">
+        <v>39</v>
+      </c>
       <c r="I69" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
@@ -3572,15 +3856,23 @@
       <c r="B70" s="8">
         <v>45</v>
       </c>
-      <c r="C70" s="8"/>
+      <c r="C70" s="8">
+        <v>1.7729000000000002E-2</v>
+      </c>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
+      <c r="F70" s="8">
+        <v>5</v>
+      </c>
+      <c r="G70" s="8">
+        <v>31</v>
+      </c>
+      <c r="H70" s="8">
+        <v>35</v>
+      </c>
       <c r="I70" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
@@ -3602,15 +3894,23 @@
       <c r="B71" s="8">
         <v>42</v>
       </c>
-      <c r="C71" s="8"/>
+      <c r="C71" s="8">
+        <v>1.1282E-2</v>
+      </c>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
+      <c r="F71" s="8">
+        <v>4</v>
+      </c>
+      <c r="G71" s="8">
+        <v>31</v>
+      </c>
+      <c r="H71" s="8">
+        <v>34</v>
+      </c>
       <c r="I71" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
@@ -3632,15 +3932,23 @@
       <c r="B72" s="8">
         <v>40</v>
       </c>
-      <c r="C72" s="8"/>
+      <c r="C72" s="8">
+        <v>8.0590000000000002E-3</v>
+      </c>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
+      <c r="F72" s="8">
+        <v>3</v>
+      </c>
+      <c r="G72" s="8">
+        <v>31</v>
+      </c>
+      <c r="H72" s="8">
+        <v>34</v>
+      </c>
       <c r="I72" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
@@ -3662,15 +3970,23 @@
       <c r="B73" s="8">
         <v>38</v>
       </c>
-      <c r="C73" s="8"/>
+      <c r="C73" s="8">
+        <v>4.0289999999999996E-3</v>
+      </c>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
+      <c r="F73" s="8">
+        <v>1</v>
+      </c>
+      <c r="G73" s="8">
+        <v>31</v>
+      </c>
+      <c r="H73" s="8">
+        <v>33</v>
+      </c>
       <c r="I73" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
@@ -3692,15 +4008,23 @@
       <c r="B74" s="8">
         <v>35</v>
       </c>
-      <c r="C74" s="8"/>
+      <c r="C74" s="8">
+        <v>0</v>
+      </c>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
+      <c r="F74" s="8">
+        <v>0</v>
+      </c>
+      <c r="G74" s="8">
+        <v>31</v>
+      </c>
+      <c r="H74" s="8">
+        <v>33</v>
+      </c>
       <c r="I74" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
@@ -3722,15 +4046,23 @@
       <c r="B75" s="8">
         <v>32</v>
       </c>
-      <c r="C75" s="8"/>
+      <c r="C75" s="8">
+        <v>0</v>
+      </c>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
+      <c r="F75" s="8">
+        <v>0</v>
+      </c>
+      <c r="G75" s="8">
+        <v>30</v>
+      </c>
+      <c r="H75" s="8">
+        <v>31</v>
+      </c>
       <c r="I75" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>30.5</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
@@ -3752,15 +4084,23 @@
       <c r="B76" s="8">
         <v>30</v>
       </c>
-      <c r="C76" s="8"/>
+      <c r="C76" s="8">
+        <v>0</v>
+      </c>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
+      <c r="F76" s="8">
+        <v>0</v>
+      </c>
+      <c r="G76" s="8">
+        <v>29</v>
+      </c>
+      <c r="H76" s="8">
+        <v>30</v>
+      </c>
       <c r="I76" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>29.5</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
@@ -3782,15 +4122,23 @@
       <c r="B77" s="8">
         <v>28</v>
       </c>
-      <c r="C77" s="8"/>
+      <c r="C77" s="8">
+        <v>0</v>
+      </c>
       <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+      <c r="E77" s="8">
+        <v>0</v>
+      </c>
       <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
+      <c r="G77" s="8">
+        <v>30</v>
+      </c>
+      <c r="H77" s="8">
+        <v>27</v>
+      </c>
       <c r="I77" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
@@ -3812,15 +4160,23 @@
       <c r="B78" s="8">
         <v>25</v>
       </c>
-      <c r="C78" s="8"/>
+      <c r="C78" s="8">
+        <v>0</v>
+      </c>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
+      <c r="F78" s="8">
+        <v>0</v>
+      </c>
+      <c r="G78" s="8">
+        <v>25</v>
+      </c>
+      <c r="H78" s="8">
+        <v>28</v>
+      </c>
       <c r="I78" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>26.5</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
@@ -3842,15 +4198,23 @@
       <c r="B79" s="9">
         <v>50</v>
       </c>
-      <c r="C79" s="9"/>
+      <c r="C79" s="9">
+        <v>1.4505000000000001E-2</v>
+      </c>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
+      <c r="F79" s="9">
+        <v>4</v>
+      </c>
+      <c r="G79" s="9">
+        <v>37</v>
+      </c>
+      <c r="H79" s="9">
+        <v>30</v>
+      </c>
       <c r="I79" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>33.5</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -3872,15 +4236,23 @@
       <c r="B80" s="9">
         <v>48</v>
       </c>
-      <c r="C80" s="9"/>
+      <c r="C80" s="9">
+        <v>1.2893999999999999E-2</v>
+      </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
+      <c r="F80" s="9">
+        <v>4</v>
+      </c>
+      <c r="G80" s="9">
+        <v>34</v>
+      </c>
+      <c r="H80" s="9">
+        <v>29</v>
+      </c>
       <c r="I80" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>31.5</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
@@ -3902,15 +4274,23 @@
       <c r="B81" s="9">
         <v>45</v>
       </c>
-      <c r="C81" s="9"/>
+      <c r="C81" s="9">
+        <v>8.8640000000000004E-3</v>
+      </c>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
+      <c r="F81" s="9">
+        <v>3</v>
+      </c>
+      <c r="G81" s="9">
+        <v>29</v>
+      </c>
+      <c r="H81" s="9">
+        <v>32</v>
+      </c>
       <c r="I81" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>30.5</v>
       </c>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
@@ -3932,15 +4312,23 @@
       <c r="B82" s="9">
         <v>42</v>
       </c>
-      <c r="C82" s="9"/>
+      <c r="C82" s="9">
+        <v>4.0259000000000003E-2</v>
+      </c>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
+      <c r="F82" s="9">
+        <v>4</v>
+      </c>
+      <c r="G82" s="9">
+        <v>28</v>
+      </c>
+      <c r="H82" s="9">
+        <v>30</v>
+      </c>
       <c r="I82" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
@@ -3962,15 +4350,23 @@
       <c r="B83" s="9">
         <v>40</v>
       </c>
-      <c r="C83" s="9"/>
+      <c r="C83" s="9">
+        <v>0</v>
+      </c>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
+      <c r="F83" s="9">
+        <v>0</v>
+      </c>
+      <c r="G83" s="9">
+        <v>27</v>
+      </c>
+      <c r="H83" s="9">
+        <v>30</v>
+      </c>
       <c r="I83" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
@@ -3992,15 +4388,23 @@
       <c r="B84" s="9">
         <v>38</v>
       </c>
-      <c r="C84" s="9"/>
+      <c r="C84" s="9">
+        <v>0</v>
+      </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
+      <c r="F84" s="9">
+        <v>0</v>
+      </c>
+      <c r="G84" s="9">
+        <v>28</v>
+      </c>
+      <c r="H84" s="9">
+        <v>29</v>
+      </c>
       <c r="I84" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
@@ -4022,15 +4426,27 @@
       <c r="B85" s="9">
         <v>35</v>
       </c>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
+      <c r="C85" s="9">
+        <v>0</v>
+      </c>
+      <c r="D85" s="9">
+        <v>0</v>
+      </c>
+      <c r="E85" s="9">
+        <v>0</v>
+      </c>
+      <c r="F85" s="9">
+        <v>0</v>
+      </c>
+      <c r="G85" s="9">
+        <v>27</v>
+      </c>
+      <c r="H85" s="9">
+        <v>28</v>
+      </c>
       <c r="I85" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
@@ -4052,15 +4468,27 @@
       <c r="B86" s="9">
         <v>32</v>
       </c>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
+      <c r="C86" s="9">
+        <v>0</v>
+      </c>
+      <c r="D86" s="9">
+        <v>0</v>
+      </c>
+      <c r="E86" s="9">
+        <v>0</v>
+      </c>
+      <c r="F86" s="9">
+        <v>0</v>
+      </c>
+      <c r="G86" s="9">
+        <v>27</v>
+      </c>
+      <c r="H86" s="9">
+        <v>28</v>
+      </c>
       <c r="I86" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
@@ -4082,15 +4510,27 @@
       <c r="B87" s="9">
         <v>30</v>
       </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
+      <c r="C87" s="9">
+        <v>0</v>
+      </c>
+      <c r="D87" s="9">
+        <v>0</v>
+      </c>
+      <c r="E87" s="9">
+        <v>0</v>
+      </c>
+      <c r="F87" s="9">
+        <v>0</v>
+      </c>
+      <c r="G87" s="9">
+        <v>21</v>
+      </c>
+      <c r="H87" s="9">
+        <v>27</v>
+      </c>
       <c r="I87" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
@@ -4112,15 +4552,27 @@
       <c r="B88" s="9">
         <v>28</v>
       </c>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
+      <c r="C88" s="9">
+        <v>0</v>
+      </c>
+      <c r="D88" s="9">
+        <v>0</v>
+      </c>
+      <c r="E88" s="9">
+        <v>0</v>
+      </c>
+      <c r="F88" s="9">
+        <v>0</v>
+      </c>
+      <c r="G88" s="9">
+        <v>24</v>
+      </c>
+      <c r="H88" s="9">
+        <v>25</v>
+      </c>
       <c r="I88" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>24.5</v>
       </c>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
@@ -4142,15 +4594,27 @@
       <c r="B89" s="9">
         <v>25</v>
       </c>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="9"/>
-      <c r="H89" s="9"/>
+      <c r="C89" s="9">
+        <v>0</v>
+      </c>
+      <c r="D89" s="9">
+        <v>0</v>
+      </c>
+      <c r="E89" s="9">
+        <v>0</v>
+      </c>
+      <c r="F89" s="9">
+        <v>0</v>
+      </c>
+      <c r="G89" s="9">
+        <v>24</v>
+      </c>
+      <c r="H89" s="9">
+        <v>25</v>
+      </c>
       <c r="I89" s="9">
         <f t="shared" ref="I89:I152" si="5">(H89+G89)/2</f>
-        <v>0</v>
+        <v>24.5</v>
       </c>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
@@ -4172,15 +4636,27 @@
       <c r="B90" s="10">
         <v>50</v>
       </c>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
+      <c r="C90" s="10">
+        <v>0</v>
+      </c>
+      <c r="D90" s="10">
+        <v>0</v>
+      </c>
+      <c r="E90" s="10">
+        <v>0</v>
+      </c>
+      <c r="F90" s="10">
+        <v>0</v>
+      </c>
+      <c r="G90" s="10">
+        <v>31</v>
+      </c>
+      <c r="H90" s="10">
+        <v>29</v>
+      </c>
       <c r="I90" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J90" s="10"/>
       <c r="K90" s="10"/>
@@ -4202,15 +4678,27 @@
       <c r="B91" s="10">
         <v>48</v>
       </c>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10"/>
-      <c r="H91" s="10"/>
+      <c r="C91" s="10">
+        <v>0</v>
+      </c>
+      <c r="D91" s="10">
+        <v>0</v>
+      </c>
+      <c r="E91" s="10">
+        <v>0</v>
+      </c>
+      <c r="F91" s="10">
+        <v>0</v>
+      </c>
+      <c r="G91" s="10">
+        <v>29</v>
+      </c>
+      <c r="H91" s="10">
+        <v>29</v>
+      </c>
       <c r="I91" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -4232,15 +4720,27 @@
       <c r="B92" s="10">
         <v>45</v>
       </c>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-      <c r="H92" s="10"/>
+      <c r="C92" s="10">
+        <v>0</v>
+      </c>
+      <c r="D92" s="10">
+        <v>0</v>
+      </c>
+      <c r="E92" s="10">
+        <v>0</v>
+      </c>
+      <c r="F92" s="10">
+        <v>0</v>
+      </c>
+      <c r="G92" s="10">
+        <v>28</v>
+      </c>
+      <c r="H92" s="10">
+        <v>25</v>
+      </c>
       <c r="I92" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>26.5</v>
       </c>
       <c r="J92" s="10"/>
       <c r="K92" s="10"/>
@@ -4262,15 +4762,27 @@
       <c r="B93" s="10">
         <v>42</v>
       </c>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
+      <c r="C93" s="10">
+        <v>0</v>
+      </c>
+      <c r="D93" s="10">
+        <v>0</v>
+      </c>
+      <c r="E93" s="10">
+        <v>0</v>
+      </c>
+      <c r="F93" s="10">
+        <v>0</v>
+      </c>
+      <c r="G93" s="10">
+        <v>28</v>
+      </c>
+      <c r="H93" s="10">
+        <v>26</v>
+      </c>
       <c r="I93" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
@@ -4292,15 +4804,27 @@
       <c r="B94" s="10">
         <v>40</v>
       </c>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
+      <c r="C94" s="10">
+        <v>0</v>
+      </c>
+      <c r="D94" s="10">
+        <v>0</v>
+      </c>
+      <c r="E94" s="10">
+        <v>0</v>
+      </c>
+      <c r="F94" s="10">
+        <v>0</v>
+      </c>
+      <c r="G94" s="10">
+        <v>26</v>
+      </c>
+      <c r="H94" s="10">
+        <v>26</v>
+      </c>
       <c r="I94" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -4322,15 +4846,27 @@
       <c r="B95" s="10">
         <v>38</v>
       </c>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
-      <c r="H95" s="10"/>
+      <c r="C95" s="10">
+        <v>0</v>
+      </c>
+      <c r="D95" s="10">
+        <v>0</v>
+      </c>
+      <c r="E95" s="10">
+        <v>0</v>
+      </c>
+      <c r="F95" s="10">
+        <v>0</v>
+      </c>
+      <c r="G95" s="10">
+        <v>25</v>
+      </c>
+      <c r="H95" s="10">
+        <v>26</v>
+      </c>
       <c r="I95" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="J95" s="10"/>
       <c r="K95" s="10"/>
@@ -4352,15 +4888,27 @@
       <c r="B96" s="10">
         <v>35</v>
       </c>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
-      <c r="H96" s="10"/>
+      <c r="C96" s="10">
+        <v>0</v>
+      </c>
+      <c r="D96" s="10">
+        <v>0</v>
+      </c>
+      <c r="E96" s="10">
+        <v>0</v>
+      </c>
+      <c r="F96" s="10">
+        <v>0</v>
+      </c>
+      <c r="G96" s="10">
+        <v>24</v>
+      </c>
+      <c r="H96" s="10">
+        <v>25</v>
+      </c>
       <c r="I96" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>24.5</v>
       </c>
       <c r="J96" s="10"/>
       <c r="K96" s="10"/>
@@ -4382,15 +4930,27 @@
       <c r="B97" s="10">
         <v>32</v>
       </c>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="10"/>
-      <c r="H97" s="10"/>
+      <c r="C97" s="10">
+        <v>0</v>
+      </c>
+      <c r="D97" s="10">
+        <v>0</v>
+      </c>
+      <c r="E97" s="10">
+        <v>0</v>
+      </c>
+      <c r="F97" s="10">
+        <v>0</v>
+      </c>
+      <c r="G97" s="10">
+        <v>23</v>
+      </c>
+      <c r="H97" s="10">
+        <v>24</v>
+      </c>
       <c r="I97" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>23.5</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -4412,15 +4972,27 @@
       <c r="B98" s="10">
         <v>30</v>
       </c>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="10"/>
-      <c r="H98" s="10"/>
+      <c r="C98" s="10">
+        <v>0</v>
+      </c>
+      <c r="D98" s="10">
+        <v>0</v>
+      </c>
+      <c r="E98" s="10">
+        <v>0</v>
+      </c>
+      <c r="F98" s="10">
+        <v>0</v>
+      </c>
+      <c r="G98" s="10">
+        <v>23</v>
+      </c>
+      <c r="H98" s="10">
+        <v>20</v>
+      </c>
       <c r="I98" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="J98" s="10"/>
       <c r="K98" s="10"/>
@@ -4442,15 +5014,27 @@
       <c r="B99" s="10">
         <v>28</v>
       </c>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="10"/>
-      <c r="H99" s="10"/>
+      <c r="C99" s="10">
+        <v>0</v>
+      </c>
+      <c r="D99" s="10">
+        <v>0</v>
+      </c>
+      <c r="E99" s="10">
+        <v>0</v>
+      </c>
+      <c r="F99" s="10">
+        <v>0</v>
+      </c>
+      <c r="G99" s="10">
+        <v>19</v>
+      </c>
+      <c r="H99" s="10">
+        <v>23</v>
+      </c>
       <c r="I99" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J99" s="10"/>
       <c r="K99" s="10"/>
@@ -4472,15 +5056,27 @@
       <c r="B100" s="10">
         <v>25</v>
       </c>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="10"/>
-      <c r="H100" s="10"/>
+      <c r="C100" s="10">
+        <v>0</v>
+      </c>
+      <c r="D100" s="10">
+        <v>0</v>
+      </c>
+      <c r="E100" s="10">
+        <v>0</v>
+      </c>
+      <c r="F100" s="10">
+        <v>0</v>
+      </c>
+      <c r="G100" s="10">
+        <v>21</v>
+      </c>
+      <c r="H100" s="10">
+        <v>21</v>
+      </c>
       <c r="I100" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -4802,12 +5398,24 @@
       <c r="B111" s="11">
         <v>25</v>
       </c>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
+      <c r="C111" s="11">
+        <v>0</v>
+      </c>
+      <c r="D111" s="11">
+        <v>0</v>
+      </c>
+      <c r="E111" s="11">
+        <v>0</v>
+      </c>
+      <c r="F111" s="11">
+        <v>0</v>
+      </c>
+      <c r="G111" s="11">
+        <v>0</v>
+      </c>
+      <c r="H111" s="11">
+        <v>0</v>
+      </c>
       <c r="I111" s="11">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4832,15 +5440,23 @@
       <c r="B112" s="2">
         <v>50</v>
       </c>
-      <c r="C112" s="2"/>
+      <c r="C112" s="2">
+        <v>1.452161</v>
+      </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
+      <c r="F112" s="2">
+        <v>355</v>
+      </c>
+      <c r="G112" s="2">
+        <v>439</v>
+      </c>
+      <c r="H112" s="2">
+        <v>408</v>
+      </c>
       <c r="I112" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>423.5</v>
       </c>
       <c r="J112" s="2">
         <v>0</v>
@@ -4862,15 +5478,23 @@
       <c r="B113" s="2">
         <v>48</v>
       </c>
-      <c r="C113" s="2"/>
+      <c r="C113" s="2">
+        <v>1.410256</v>
+      </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
+      <c r="F113" s="2">
+        <v>355</v>
+      </c>
+      <c r="G113" s="2">
+        <v>409</v>
+      </c>
+      <c r="H113" s="2">
+        <v>414</v>
+      </c>
       <c r="I113" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>411.5</v>
       </c>
       <c r="J113" s="2">
         <v>0</v>
@@ -4892,15 +5516,23 @@
       <c r="B114" s="2">
         <v>45</v>
       </c>
-      <c r="C114" s="2"/>
+      <c r="C114" s="2">
+        <v>1.349817</v>
+      </c>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
+      <c r="F114" s="2">
+        <v>354</v>
+      </c>
+      <c r="G114" s="2">
+        <v>393</v>
+      </c>
+      <c r="H114" s="2">
+        <v>386</v>
+      </c>
       <c r="I114" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>389.5</v>
       </c>
       <c r="J114" s="2">
         <v>0</v>
@@ -4922,15 +5554,23 @@
       <c r="B115" s="2">
         <v>42</v>
       </c>
-      <c r="C115" s="2"/>
+      <c r="C115" s="2">
+        <v>1.293407</v>
+      </c>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
+      <c r="F115" s="2">
+        <v>354</v>
+      </c>
+      <c r="G115" s="2">
+        <v>379</v>
+      </c>
+      <c r="H115" s="2">
+        <v>384</v>
+      </c>
       <c r="I115" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>381.5</v>
       </c>
       <c r="J115" s="2">
         <v>0</v>
@@ -4952,15 +5592,23 @@
       <c r="B116" s="2">
         <v>40</v>
       </c>
-      <c r="C116" s="2"/>
+      <c r="C116" s="2">
+        <v>1.2369300000000001</v>
+      </c>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
+      <c r="F116" s="2">
+        <v>350</v>
+      </c>
+      <c r="G116" s="2">
+        <v>387</v>
+      </c>
+      <c r="H116" s="2">
+        <v>363</v>
+      </c>
       <c r="I116" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="J116" s="2">
         <v>0</v>
@@ -4982,15 +5630,23 @@
       <c r="B117" s="2">
         <v>38</v>
       </c>
-      <c r="C117" s="2"/>
+      <c r="C117" s="2">
+        <v>1.2023440000000001</v>
+      </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
+      <c r="F117" s="2">
+        <v>351</v>
+      </c>
+      <c r="G117" s="2">
+        <v>395</v>
+      </c>
+      <c r="H117" s="2">
+        <v>357</v>
+      </c>
       <c r="I117" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="J117" s="2">
         <v>0</v>
@@ -5012,15 +5668,23 @@
       <c r="B118" s="2">
         <v>35</v>
       </c>
-      <c r="C118" s="2"/>
+      <c r="C118" s="2">
+        <v>1.1394869999999999</v>
+      </c>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
+      <c r="F118" s="2">
+        <v>349</v>
+      </c>
+      <c r="G118" s="2">
+        <v>385</v>
+      </c>
+      <c r="H118" s="2">
+        <v>337</v>
+      </c>
       <c r="I118" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="J118" s="2">
         <v>0</v>
@@ -5042,15 +5706,23 @@
       <c r="B119" s="2">
         <v>32</v>
       </c>
-      <c r="C119" s="2"/>
+      <c r="C119" s="2">
+        <v>1.070989</v>
+      </c>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
+      <c r="F119" s="2">
+        <v>345</v>
+      </c>
+      <c r="G119" s="2">
+        <v>382</v>
+      </c>
+      <c r="H119" s="2">
+        <v>333</v>
+      </c>
       <c r="I119" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>357.5</v>
       </c>
       <c r="J119" s="2">
         <v>0</v>
@@ -5072,15 +5744,23 @@
       <c r="B120" s="2">
         <v>30</v>
       </c>
-      <c r="C120" s="2"/>
+      <c r="C120" s="2">
+        <v>1.033919</v>
+      </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
+      <c r="F120" s="2">
+        <v>345</v>
+      </c>
+      <c r="G120" s="2">
+        <v>324</v>
+      </c>
+      <c r="H120" s="2">
+        <v>376</v>
+      </c>
       <c r="I120" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="J120" s="2">
         <v>0</v>
@@ -5102,15 +5782,23 @@
       <c r="B121" s="2">
         <v>28</v>
       </c>
-      <c r="C121" s="2"/>
+      <c r="C121" s="2">
+        <v>0.99201499999999998</v>
+      </c>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
+      <c r="F121" s="2">
+        <v>344</v>
+      </c>
+      <c r="G121" s="2">
+        <v>311</v>
+      </c>
+      <c r="H121" s="2">
+        <v>372</v>
+      </c>
       <c r="I121" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>341.5</v>
       </c>
       <c r="J121" s="2">
         <v>0</v>
@@ -5132,15 +5820,23 @@
       <c r="B122" s="2">
         <v>25</v>
       </c>
-      <c r="C122" s="2"/>
+      <c r="C122" s="2">
+        <v>0.93640999999999996</v>
+      </c>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
+      <c r="F122" s="2">
+        <v>344</v>
+      </c>
+      <c r="G122" s="2">
+        <v>362</v>
+      </c>
+      <c r="H122" s="2">
+        <v>302</v>
+      </c>
       <c r="I122" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>332</v>
       </c>
       <c r="J122" s="2">
         <v>0</v>
@@ -12397,10 +13093,12 @@
       <c r="E364" s="17"/>
       <c r="F364" s="17"/>
       <c r="G364" s="17"/>
-      <c r="H364" s="17"/>
+      <c r="H364" s="17">
+        <v>12</v>
+      </c>
       <c r="I364" s="17">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f>(H364+G364)/2</f>
+        <v>6</v>
       </c>
       <c r="J364" s="17">
         <v>3</v>

</xml_diff>

<commit_message>
Revert "Data as on 9-1-21-Morning"
This reverts commit 9d95c83f21137ca433ce6381c2dcc333bdeccad9.
</commit_message>
<xml_diff>
--- a/0. Files/1. Water Quality/5. Data/2. Calibration/TDS-Data.xlsx
+++ b/0. Files/1. Water Quality/5. Data/2. Calibration/TDS-Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Jupyter Notebooks\Projects\WaterDataAnalysis\0. Files\1. Water Quality\5. Data\2. Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Desktop\Files\1. Projects\1. Water Quality\5. Data\2. Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41DAC68-5CA8-4ED3-8413-8470A8BC4E25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CD0987-6F71-4F72-9D47-9C825B0CC80A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:N364"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1197,7 @@
         <v>91</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I11" si="0">(G3+H3)/2</f>
+        <f t="shared" ref="I3:I12" si="0">(G3+H3)/2</f>
         <v>91</v>
       </c>
       <c r="J3" s="2"/>
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="2">
-        <f>(126*100*J7+332*100*K7+70*L7*100)/(100*J7+100*K7+L7*100+M7*100)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="2">
-        <f>(126*100*J9+324*100*K9+70*L9*100)/(100*J9+100*K9+L9*100+M9*100)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -1503,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <f>(126*100*J10+324*100*K10+70*L10*100)/(100*J10+100*K10+L10*100+M10*100)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
         <v>82</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" ref="I14:I22" si="2">(H14+G14)/2</f>
+        <f t="shared" ref="I14:I23" si="2">(H14+G14)/2</f>
         <v>81</v>
       </c>
       <c r="J14" s="3"/>
@@ -2522,23 +2522,15 @@
       <c r="B35" s="5">
         <v>50</v>
       </c>
-      <c r="C35" s="5">
-        <v>7.8974000000000003E-2</v>
-      </c>
+      <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="5">
-        <v>22</v>
-      </c>
-      <c r="G35" s="5">
-        <v>56</v>
-      </c>
-      <c r="H35" s="5">
-        <v>46</v>
-      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
       <c r="I35" s="5">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -2560,23 +2552,15 @@
       <c r="B36" s="5">
         <v>48</v>
       </c>
-      <c r="C36" s="5">
-        <v>7.4138999999999997E-2</v>
-      </c>
+      <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="5">
-        <v>21</v>
-      </c>
-      <c r="G36" s="5">
-        <v>49</v>
-      </c>
-      <c r="H36" s="5">
-        <v>45</v>
-      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="5">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -2598,23 +2582,15 @@
       <c r="B37" s="5">
         <v>45</v>
       </c>
-      <c r="C37" s="5">
-        <v>6.4468999999999999E-2</v>
-      </c>
+      <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="5">
-        <v>19</v>
-      </c>
-      <c r="G37" s="5">
-        <v>46</v>
-      </c>
-      <c r="H37" s="5">
-        <v>45</v>
-      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
       <c r="I37" s="5">
         <f t="shared" si="3"/>
-        <v>45.5</v>
+        <v>0</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -2636,23 +2612,15 @@
       <c r="B38" s="5">
         <v>42</v>
       </c>
-      <c r="C38" s="5">
-        <v>5.6410000000000002E-2</v>
-      </c>
+      <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="5">
-        <v>18</v>
-      </c>
-      <c r="G38" s="5">
-        <v>45</v>
-      </c>
-      <c r="H38" s="5">
-        <v>47</v>
-      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
       <c r="I38" s="5">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
@@ -2674,23 +2642,15 @@
       <c r="B39" s="5">
         <v>40</v>
       </c>
-      <c r="C39" s="5">
-        <v>5.1575000000000003E-2</v>
-      </c>
+      <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
-      <c r="F39" s="5">
-        <v>17</v>
-      </c>
-      <c r="G39" s="5">
-        <v>45</v>
-      </c>
-      <c r="H39" s="5">
-        <v>45</v>
-      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
       <c r="I39" s="5">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
@@ -2712,23 +2672,15 @@
       <c r="B40" s="5">
         <v>38</v>
       </c>
-      <c r="C40" s="5">
-        <v>4.7545999999999998E-2</v>
-      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="5">
-        <v>16</v>
-      </c>
-      <c r="G40" s="5">
-        <v>47</v>
-      </c>
-      <c r="H40" s="5">
-        <v>45</v>
-      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
       <c r="I40" s="5">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -2750,23 +2702,15 @@
       <c r="B41" s="5">
         <v>35</v>
       </c>
-      <c r="C41" s="5">
-        <v>3.9487000000000001E-2</v>
-      </c>
+      <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="5">
-        <v>14</v>
-      </c>
-      <c r="G41" s="5">
-        <v>45</v>
-      </c>
-      <c r="H41" s="5">
-        <v>46</v>
-      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
       <c r="I41" s="5">
         <f t="shared" si="3"/>
-        <v>45.5</v>
+        <v>0</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
@@ -2788,23 +2732,15 @@
       <c r="B42" s="5">
         <v>32</v>
       </c>
-      <c r="C42" s="5">
-        <v>3.304E-2</v>
-      </c>
+      <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="5">
-        <v>12</v>
-      </c>
-      <c r="G42" s="5">
-        <v>45</v>
-      </c>
-      <c r="H42" s="5">
-        <v>45</v>
-      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
       <c r="I42" s="5">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
@@ -2826,23 +2762,15 @@
       <c r="B43" s="5">
         <v>30</v>
       </c>
-      <c r="C43" s="5">
-        <v>2.6592999999999999E-2</v>
-      </c>
+      <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="5">
-        <v>10</v>
-      </c>
-      <c r="G43" s="5">
-        <v>44</v>
-      </c>
-      <c r="H43" s="5">
-        <v>39</v>
-      </c>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
       <c r="I43" s="5">
         <f t="shared" si="3"/>
-        <v>41.5</v>
+        <v>0</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
@@ -2864,23 +2792,15 @@
       <c r="B44" s="5">
         <v>28</v>
       </c>
-      <c r="C44" s="5">
-        <v>2.2564000000000001E-2</v>
-      </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="5">
-        <v>9</v>
-      </c>
-      <c r="G44" s="5">
-        <v>45</v>
-      </c>
-      <c r="H44" s="5">
-        <v>42</v>
-      </c>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
       <c r="I44" s="5">
         <f t="shared" si="3"/>
-        <v>43.5</v>
+        <v>0</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
@@ -2902,23 +2822,15 @@
       <c r="B45" s="5">
         <v>25</v>
       </c>
-      <c r="C45" s="5">
-        <v>1.5311E-2</v>
-      </c>
+      <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="5">
-        <v>7</v>
-      </c>
-      <c r="G45" s="5">
-        <v>40</v>
-      </c>
-      <c r="H45" s="5">
-        <v>44</v>
-      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
       <c r="I45" s="5">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
@@ -2940,23 +2852,15 @@
       <c r="B46" s="6">
         <v>50</v>
       </c>
-      <c r="C46" s="6">
-        <v>5.8021999999999997E-2</v>
-      </c>
+      <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
-      <c r="F46" s="6">
-        <v>16</v>
-      </c>
-      <c r="G46" s="6">
-        <v>40</v>
-      </c>
-      <c r="H46" s="6">
-        <v>46</v>
-      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
       <c r="I46" s="6">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -2978,23 +2882,15 @@
       <c r="B47" s="6">
         <v>48</v>
       </c>
-      <c r="C47" s="6">
-        <v>5.3186999999999998E-2</v>
-      </c>
+      <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
-      <c r="F47" s="6">
-        <v>15</v>
-      </c>
-      <c r="G47" s="6">
-        <v>43</v>
-      </c>
-      <c r="H47" s="6">
-        <v>39</v>
-      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
       <c r="I47" s="6">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -3016,23 +2912,15 @@
       <c r="B48" s="6">
         <v>45</v>
       </c>
-      <c r="C48" s="6">
-        <v>4.7545999999999998E-2</v>
-      </c>
+      <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
-      <c r="F48" s="6">
-        <v>14</v>
-      </c>
-      <c r="G48" s="6">
-        <v>45</v>
-      </c>
-      <c r="H48" s="6">
-        <v>40</v>
-      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
       <c r="I48" s="6">
         <f t="shared" si="3"/>
-        <v>42.5</v>
+        <v>0</v>
       </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -3054,23 +2942,15 @@
       <c r="B49" s="6">
         <v>42</v>
       </c>
-      <c r="C49" s="6">
-        <v>3.8681E-2</v>
-      </c>
+      <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
-      <c r="F49" s="6">
-        <v>12</v>
-      </c>
-      <c r="G49" s="6">
-        <v>44</v>
-      </c>
-      <c r="H49" s="6">
-        <v>45</v>
-      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
       <c r="I49" s="6">
         <f t="shared" si="3"/>
-        <v>44.5</v>
+        <v>0</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -3092,23 +2972,15 @@
       <c r="B50" s="6">
         <v>40</v>
       </c>
-      <c r="C50" s="6">
-        <v>3.7874999999999999E-2</v>
-      </c>
+      <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="6">
-        <v>12</v>
-      </c>
-      <c r="G50" s="6">
-        <v>40</v>
-      </c>
-      <c r="H50" s="6">
-        <v>44</v>
-      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
       <c r="I50" s="6">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -3130,23 +3002,15 @@
       <c r="B51" s="6">
         <v>38</v>
       </c>
-      <c r="C51" s="6">
-        <v>3.3846000000000001E-2</v>
-      </c>
+      <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
-      <c r="F51" s="6">
-        <v>11</v>
-      </c>
-      <c r="G51" s="6">
-        <v>43</v>
-      </c>
-      <c r="H51" s="6">
-        <v>40</v>
-      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
       <c r="I51" s="6">
         <f t="shared" si="3"/>
-        <v>41.5</v>
+        <v>0</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -3168,23 +3032,15 @@
       <c r="B52" s="6">
         <v>35</v>
       </c>
-      <c r="C52" s="6">
-        <v>2.4982000000000001E-2</v>
-      </c>
+      <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
-      <c r="F52" s="6">
-        <v>9</v>
-      </c>
-      <c r="G52" s="6">
-        <v>40</v>
-      </c>
-      <c r="H52" s="6">
-        <v>41</v>
-      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
       <c r="I52" s="6">
         <f t="shared" si="3"/>
-        <v>40.5</v>
+        <v>0</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -3206,23 +3062,15 @@
       <c r="B53" s="6">
         <v>32</v>
       </c>
-      <c r="C53" s="6">
-        <v>1.8534999999999999E-2</v>
-      </c>
+      <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
-      <c r="F53" s="6">
-        <v>7</v>
-      </c>
-      <c r="G53" s="6">
-        <v>41</v>
-      </c>
-      <c r="H53" s="6">
-        <v>41</v>
-      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
       <c r="I53" s="6">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -3244,23 +3092,15 @@
       <c r="B54" s="6">
         <v>30</v>
       </c>
-      <c r="C54" s="6">
-        <v>1.37E-2</v>
-      </c>
+      <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="6">
-        <v>5</v>
-      </c>
-      <c r="G54" s="6">
-        <v>38</v>
-      </c>
-      <c r="H54" s="6">
-        <v>40</v>
-      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
       <c r="I54" s="6">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -3282,23 +3122,15 @@
       <c r="B55" s="6">
         <v>28</v>
       </c>
-      <c r="C55" s="6">
-        <v>1.1282E-2</v>
-      </c>
+      <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
-      <c r="F55" s="6">
-        <v>5</v>
-      </c>
-      <c r="G55" s="6">
-        <v>38</v>
-      </c>
-      <c r="H55" s="6">
-        <v>40</v>
-      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
       <c r="I55" s="6">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -3320,23 +3152,15 @@
       <c r="B56" s="6">
         <v>25</v>
       </c>
-      <c r="C56" s="6">
-        <v>0</v>
-      </c>
+      <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
-      <c r="F56" s="6">
-        <v>0</v>
-      </c>
-      <c r="G56" s="6">
-        <v>35</v>
-      </c>
-      <c r="H56" s="6">
-        <v>39</v>
-      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
       <c r="I56" s="6">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -3358,23 +3182,15 @@
       <c r="B57" s="7">
         <v>50</v>
       </c>
-      <c r="C57" s="7">
-        <v>5.1575000000000003E-2</v>
-      </c>
+      <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
-      <c r="F57" s="7">
-        <v>15</v>
-      </c>
-      <c r="G57" s="7">
-        <v>39</v>
-      </c>
-      <c r="H57" s="7">
-        <v>46</v>
-      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
       <c r="I57" s="7">
         <f t="shared" si="3"/>
-        <v>42.5</v>
+        <v>0</v>
       </c>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
@@ -3396,23 +3212,15 @@
       <c r="B58" s="7">
         <v>48</v>
       </c>
-      <c r="C58" s="7">
-        <v>4.5934000000000003E-2</v>
-      </c>
+      <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="7">
-        <v>13</v>
-      </c>
-      <c r="G58" s="7">
-        <v>43</v>
-      </c>
-      <c r="H58" s="7">
-        <v>39</v>
-      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
       <c r="I58" s="7">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
@@ -3434,23 +3242,15 @@
       <c r="B59" s="7">
         <v>45</v>
       </c>
-      <c r="C59" s="7">
-        <v>3.8681E-2</v>
-      </c>
+      <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
-      <c r="F59" s="7">
-        <v>12</v>
-      </c>
-      <c r="G59" s="7">
-        <v>39</v>
-      </c>
-      <c r="H59" s="7">
-        <v>43</v>
-      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
       <c r="I59" s="7">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
@@ -3472,23 +3272,15 @@
       <c r="B60" s="7">
         <v>42</v>
       </c>
-      <c r="C60" s="7">
-        <v>3.304E-2</v>
-      </c>
+      <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
-      <c r="F60" s="7">
-        <v>10</v>
-      </c>
-      <c r="G60" s="7">
-        <v>37</v>
-      </c>
-      <c r="H60" s="7">
-        <v>43</v>
-      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
       <c r="I60" s="7">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
@@ -3510,23 +3302,15 @@
       <c r="B61" s="7">
         <v>40</v>
       </c>
-      <c r="C61" s="7">
-        <v>2.8205000000000001E-2</v>
-      </c>
+      <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="7">
-        <v>9</v>
-      </c>
-      <c r="G61" s="7">
-        <v>38</v>
-      </c>
-      <c r="H61" s="7">
-        <v>41</v>
-      </c>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
       <c r="I61" s="7">
         <f t="shared" si="3"/>
-        <v>39.5</v>
+        <v>0</v>
       </c>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
@@ -3548,23 +3332,15 @@
       <c r="B62" s="7">
         <v>38</v>
       </c>
-      <c r="C62" s="7">
-        <v>2.4982000000000001E-2</v>
-      </c>
+      <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
-      <c r="F62" s="7">
-        <v>8</v>
-      </c>
-      <c r="G62" s="7">
-        <v>38</v>
-      </c>
-      <c r="H62" s="7">
-        <v>39</v>
-      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
       <c r="I62" s="7">
         <f t="shared" si="3"/>
-        <v>38.5</v>
+        <v>0</v>
       </c>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
@@ -3586,23 +3362,15 @@
       <c r="B63" s="7">
         <v>35</v>
       </c>
-      <c r="C63" s="7">
-        <v>1.6923000000000001E-2</v>
-      </c>
+      <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
-      <c r="F63" s="7">
-        <v>6</v>
-      </c>
-      <c r="G63" s="7">
-        <v>38</v>
-      </c>
-      <c r="H63" s="7">
-        <v>39</v>
-      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
       <c r="I63" s="7">
         <f t="shared" si="3"/>
-        <v>38.5</v>
+        <v>0</v>
       </c>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
@@ -3624,23 +3392,15 @@
       <c r="B64" s="7">
         <v>32</v>
       </c>
-      <c r="C64" s="7">
-        <v>1.2893999999999999E-2</v>
-      </c>
+      <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="7">
-        <v>5</v>
-      </c>
-      <c r="G64" s="7">
-        <v>38</v>
-      </c>
-      <c r="H64" s="7">
-        <v>38</v>
-      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
       <c r="I64" s="7">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
@@ -3662,23 +3422,15 @@
       <c r="B65" s="7">
         <v>30</v>
       </c>
-      <c r="C65" s="7">
-        <v>5.6410000000000002E-3</v>
-      </c>
+      <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="7">
-        <v>2</v>
-      </c>
-      <c r="G65" s="7">
-        <v>37</v>
-      </c>
-      <c r="H65" s="7">
-        <v>38</v>
-      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
       <c r="I65" s="7">
         <f t="shared" si="3"/>
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
@@ -3700,23 +3452,15 @@
       <c r="B66" s="7">
         <v>28</v>
       </c>
-      <c r="C66" s="7">
-        <v>1.6119999999999999E-3</v>
-      </c>
+      <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
-      <c r="F66" s="7">
-        <v>1</v>
-      </c>
-      <c r="G66" s="7">
-        <v>35</v>
-      </c>
-      <c r="H66" s="7">
-        <v>38</v>
-      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
       <c r="I66" s="7">
         <f t="shared" si="3"/>
-        <v>36.5</v>
+        <v>0</v>
       </c>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
@@ -3738,27 +3482,15 @@
       <c r="B67" s="7">
         <v>25</v>
       </c>
-      <c r="C67" s="7">
-        <v>0</v>
-      </c>
-      <c r="D67" s="7">
-        <v>0</v>
-      </c>
-      <c r="E67" s="7">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7">
-        <v>0</v>
-      </c>
-      <c r="G67" s="7">
-        <v>31</v>
-      </c>
-      <c r="H67" s="7">
-        <v>36</v>
-      </c>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
       <c r="I67" s="7">
         <f t="shared" si="3"/>
-        <v>33.5</v>
+        <v>0</v>
       </c>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
@@ -3780,23 +3512,15 @@
       <c r="B68" s="8">
         <v>50</v>
       </c>
-      <c r="C68" s="8">
-        <v>2.9817E-2</v>
-      </c>
+      <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
-      <c r="F68" s="8">
-        <v>8</v>
-      </c>
-      <c r="G68" s="8">
-        <v>42</v>
-      </c>
-      <c r="H68" s="8">
-        <v>33</v>
-      </c>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
       <c r="I68" s="8">
         <f t="shared" si="3"/>
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="8"/>
@@ -3818,23 +3542,15 @@
       <c r="B69" s="8">
         <v>48</v>
       </c>
-      <c r="C69" s="8">
-        <v>2.4176E-2</v>
-      </c>
+      <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
-      <c r="F69" s="8">
-        <v>7</v>
-      </c>
-      <c r="G69" s="8">
-        <v>33</v>
-      </c>
-      <c r="H69" s="8">
-        <v>39</v>
-      </c>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
       <c r="I69" s="8">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
@@ -3856,23 +3572,15 @@
       <c r="B70" s="8">
         <v>45</v>
       </c>
-      <c r="C70" s="8">
-        <v>1.7729000000000002E-2</v>
-      </c>
+      <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
-      <c r="F70" s="8">
-        <v>5</v>
-      </c>
-      <c r="G70" s="8">
-        <v>31</v>
-      </c>
-      <c r="H70" s="8">
-        <v>35</v>
-      </c>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
       <c r="I70" s="8">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
@@ -3894,23 +3602,15 @@
       <c r="B71" s="8">
         <v>42</v>
       </c>
-      <c r="C71" s="8">
-        <v>1.1282E-2</v>
-      </c>
+      <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
-      <c r="F71" s="8">
-        <v>4</v>
-      </c>
-      <c r="G71" s="8">
-        <v>31</v>
-      </c>
-      <c r="H71" s="8">
-        <v>34</v>
-      </c>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
       <c r="I71" s="8">
         <f t="shared" si="3"/>
-        <v>32.5</v>
+        <v>0</v>
       </c>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
@@ -3932,23 +3632,15 @@
       <c r="B72" s="8">
         <v>40</v>
       </c>
-      <c r="C72" s="8">
-        <v>8.0590000000000002E-3</v>
-      </c>
+      <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
-      <c r="F72" s="8">
-        <v>3</v>
-      </c>
-      <c r="G72" s="8">
-        <v>31</v>
-      </c>
-      <c r="H72" s="8">
-        <v>34</v>
-      </c>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
       <c r="I72" s="8">
         <f t="shared" si="3"/>
-        <v>32.5</v>
+        <v>0</v>
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
@@ -3970,23 +3662,15 @@
       <c r="B73" s="8">
         <v>38</v>
       </c>
-      <c r="C73" s="8">
-        <v>4.0289999999999996E-3</v>
-      </c>
+      <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
-      <c r="F73" s="8">
-        <v>1</v>
-      </c>
-      <c r="G73" s="8">
-        <v>31</v>
-      </c>
-      <c r="H73" s="8">
-        <v>33</v>
-      </c>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
       <c r="I73" s="8">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
@@ -4008,23 +3692,15 @@
       <c r="B74" s="8">
         <v>35</v>
       </c>
-      <c r="C74" s="8">
-        <v>0</v>
-      </c>
+      <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
-      <c r="F74" s="8">
-        <v>0</v>
-      </c>
-      <c r="G74" s="8">
-        <v>31</v>
-      </c>
-      <c r="H74" s="8">
-        <v>33</v>
-      </c>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
       <c r="I74" s="8">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
@@ -4046,23 +3722,15 @@
       <c r="B75" s="8">
         <v>32</v>
       </c>
-      <c r="C75" s="8">
-        <v>0</v>
-      </c>
+      <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
-      <c r="F75" s="8">
-        <v>0</v>
-      </c>
-      <c r="G75" s="8">
-        <v>30</v>
-      </c>
-      <c r="H75" s="8">
-        <v>31</v>
-      </c>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
       <c r="I75" s="8">
         <f t="shared" si="3"/>
-        <v>30.5</v>
+        <v>0</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
@@ -4084,23 +3752,15 @@
       <c r="B76" s="8">
         <v>30</v>
       </c>
-      <c r="C76" s="8">
-        <v>0</v>
-      </c>
+      <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
-      <c r="F76" s="8">
-        <v>0</v>
-      </c>
-      <c r="G76" s="8">
-        <v>29</v>
-      </c>
-      <c r="H76" s="8">
-        <v>30</v>
-      </c>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
       <c r="I76" s="8">
         <f t="shared" si="3"/>
-        <v>29.5</v>
+        <v>0</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
@@ -4122,23 +3782,15 @@
       <c r="B77" s="8">
         <v>28</v>
       </c>
-      <c r="C77" s="8">
-        <v>0</v>
-      </c>
+      <c r="C77" s="8"/>
       <c r="D77" s="8"/>
-      <c r="E77" s="8">
-        <v>0</v>
-      </c>
+      <c r="E77" s="8"/>
       <c r="F77" s="8"/>
-      <c r="G77" s="8">
-        <v>30</v>
-      </c>
-      <c r="H77" s="8">
-        <v>27</v>
-      </c>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
       <c r="I77" s="8">
         <f t="shared" si="3"/>
-        <v>28.5</v>
+        <v>0</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
@@ -4160,23 +3812,15 @@
       <c r="B78" s="8">
         <v>25</v>
       </c>
-      <c r="C78" s="8">
-        <v>0</v>
-      </c>
+      <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
-      <c r="F78" s="8">
-        <v>0</v>
-      </c>
-      <c r="G78" s="8">
-        <v>25</v>
-      </c>
-      <c r="H78" s="8">
-        <v>28</v>
-      </c>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
       <c r="I78" s="8">
         <f t="shared" si="3"/>
-        <v>26.5</v>
+        <v>0</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
@@ -4198,23 +3842,15 @@
       <c r="B79" s="9">
         <v>50</v>
       </c>
-      <c r="C79" s="9">
-        <v>1.4505000000000001E-2</v>
-      </c>
+      <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
-      <c r="F79" s="9">
-        <v>4</v>
-      </c>
-      <c r="G79" s="9">
-        <v>37</v>
-      </c>
-      <c r="H79" s="9">
-        <v>30</v>
-      </c>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
       <c r="I79" s="9">
         <f t="shared" si="3"/>
-        <v>33.5</v>
+        <v>0</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -4236,23 +3872,15 @@
       <c r="B80" s="9">
         <v>48</v>
       </c>
-      <c r="C80" s="9">
-        <v>1.2893999999999999E-2</v>
-      </c>
+      <c r="C80" s="9"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
-      <c r="F80" s="9">
-        <v>4</v>
-      </c>
-      <c r="G80" s="9">
-        <v>34</v>
-      </c>
-      <c r="H80" s="9">
-        <v>29</v>
-      </c>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
       <c r="I80" s="9">
         <f t="shared" si="3"/>
-        <v>31.5</v>
+        <v>0</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
@@ -4274,23 +3902,15 @@
       <c r="B81" s="9">
         <v>45</v>
       </c>
-      <c r="C81" s="9">
-        <v>8.8640000000000004E-3</v>
-      </c>
+      <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
-      <c r="F81" s="9">
-        <v>3</v>
-      </c>
-      <c r="G81" s="9">
-        <v>29</v>
-      </c>
-      <c r="H81" s="9">
-        <v>32</v>
-      </c>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
       <c r="I81" s="9">
         <f t="shared" si="3"/>
-        <v>30.5</v>
+        <v>0</v>
       </c>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
@@ -4312,23 +3932,15 @@
       <c r="B82" s="9">
         <v>42</v>
       </c>
-      <c r="C82" s="9">
-        <v>4.0259000000000003E-2</v>
-      </c>
+      <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
-      <c r="F82" s="9">
-        <v>4</v>
-      </c>
-      <c r="G82" s="9">
-        <v>28</v>
-      </c>
-      <c r="H82" s="9">
-        <v>30</v>
-      </c>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
       <c r="I82" s="9">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
@@ -4350,23 +3962,15 @@
       <c r="B83" s="9">
         <v>40</v>
       </c>
-      <c r="C83" s="9">
-        <v>0</v>
-      </c>
+      <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
-      <c r="F83" s="9">
-        <v>0</v>
-      </c>
-      <c r="G83" s="9">
-        <v>27</v>
-      </c>
-      <c r="H83" s="9">
-        <v>30</v>
-      </c>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
       <c r="I83" s="9">
         <f t="shared" si="3"/>
-        <v>28.5</v>
+        <v>0</v>
       </c>
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
@@ -4388,23 +3992,15 @@
       <c r="B84" s="9">
         <v>38</v>
       </c>
-      <c r="C84" s="9">
-        <v>0</v>
-      </c>
+      <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
-      <c r="F84" s="9">
-        <v>0</v>
-      </c>
-      <c r="G84" s="9">
-        <v>28</v>
-      </c>
-      <c r="H84" s="9">
-        <v>29</v>
-      </c>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
       <c r="I84" s="9">
         <f t="shared" si="3"/>
-        <v>28.5</v>
+        <v>0</v>
       </c>
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
@@ -4426,27 +4022,15 @@
       <c r="B85" s="9">
         <v>35</v>
       </c>
-      <c r="C85" s="9">
-        <v>0</v>
-      </c>
-      <c r="D85" s="9">
-        <v>0</v>
-      </c>
-      <c r="E85" s="9">
-        <v>0</v>
-      </c>
-      <c r="F85" s="9">
-        <v>0</v>
-      </c>
-      <c r="G85" s="9">
-        <v>27</v>
-      </c>
-      <c r="H85" s="9">
-        <v>28</v>
-      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
       <c r="I85" s="9">
         <f t="shared" si="3"/>
-        <v>27.5</v>
+        <v>0</v>
       </c>
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
@@ -4468,27 +4052,15 @@
       <c r="B86" s="9">
         <v>32</v>
       </c>
-      <c r="C86" s="9">
-        <v>0</v>
-      </c>
-      <c r="D86" s="9">
-        <v>0</v>
-      </c>
-      <c r="E86" s="9">
-        <v>0</v>
-      </c>
-      <c r="F86" s="9">
-        <v>0</v>
-      </c>
-      <c r="G86" s="9">
-        <v>27</v>
-      </c>
-      <c r="H86" s="9">
-        <v>28</v>
-      </c>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
       <c r="I86" s="9">
         <f t="shared" si="3"/>
-        <v>27.5</v>
+        <v>0</v>
       </c>
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
@@ -4510,27 +4082,15 @@
       <c r="B87" s="9">
         <v>30</v>
       </c>
-      <c r="C87" s="9">
-        <v>0</v>
-      </c>
-      <c r="D87" s="9">
-        <v>0</v>
-      </c>
-      <c r="E87" s="9">
-        <v>0</v>
-      </c>
-      <c r="F87" s="9">
-        <v>0</v>
-      </c>
-      <c r="G87" s="9">
-        <v>21</v>
-      </c>
-      <c r="H87" s="9">
-        <v>27</v>
-      </c>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
       <c r="I87" s="9">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
@@ -4552,27 +4112,15 @@
       <c r="B88" s="9">
         <v>28</v>
       </c>
-      <c r="C88" s="9">
-        <v>0</v>
-      </c>
-      <c r="D88" s="9">
-        <v>0</v>
-      </c>
-      <c r="E88" s="9">
-        <v>0</v>
-      </c>
-      <c r="F88" s="9">
-        <v>0</v>
-      </c>
-      <c r="G88" s="9">
-        <v>24</v>
-      </c>
-      <c r="H88" s="9">
-        <v>25</v>
-      </c>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
       <c r="I88" s="9">
         <f t="shared" si="3"/>
-        <v>24.5</v>
+        <v>0</v>
       </c>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
@@ -4594,27 +4142,15 @@
       <c r="B89" s="9">
         <v>25</v>
       </c>
-      <c r="C89" s="9">
-        <v>0</v>
-      </c>
-      <c r="D89" s="9">
-        <v>0</v>
-      </c>
-      <c r="E89" s="9">
-        <v>0</v>
-      </c>
-      <c r="F89" s="9">
-        <v>0</v>
-      </c>
-      <c r="G89" s="9">
-        <v>24</v>
-      </c>
-      <c r="H89" s="9">
-        <v>25</v>
-      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
       <c r="I89" s="9">
         <f t="shared" ref="I89:I152" si="5">(H89+G89)/2</f>
-        <v>24.5</v>
+        <v>0</v>
       </c>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
@@ -4636,27 +4172,15 @@
       <c r="B90" s="10">
         <v>50</v>
       </c>
-      <c r="C90" s="10">
-        <v>0</v>
-      </c>
-      <c r="D90" s="10">
-        <v>0</v>
-      </c>
-      <c r="E90" s="10">
-        <v>0</v>
-      </c>
-      <c r="F90" s="10">
-        <v>0</v>
-      </c>
-      <c r="G90" s="10">
-        <v>31</v>
-      </c>
-      <c r="H90" s="10">
-        <v>29</v>
-      </c>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
       <c r="I90" s="10">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J90" s="10"/>
       <c r="K90" s="10"/>
@@ -4678,27 +4202,15 @@
       <c r="B91" s="10">
         <v>48</v>
       </c>
-      <c r="C91" s="10">
-        <v>0</v>
-      </c>
-      <c r="D91" s="10">
-        <v>0</v>
-      </c>
-      <c r="E91" s="10">
-        <v>0</v>
-      </c>
-      <c r="F91" s="10">
-        <v>0</v>
-      </c>
-      <c r="G91" s="10">
-        <v>29</v>
-      </c>
-      <c r="H91" s="10">
-        <v>29</v>
-      </c>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
       <c r="I91" s="10">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -4720,27 +4232,15 @@
       <c r="B92" s="10">
         <v>45</v>
       </c>
-      <c r="C92" s="10">
-        <v>0</v>
-      </c>
-      <c r="D92" s="10">
-        <v>0</v>
-      </c>
-      <c r="E92" s="10">
-        <v>0</v>
-      </c>
-      <c r="F92" s="10">
-        <v>0</v>
-      </c>
-      <c r="G92" s="10">
-        <v>28</v>
-      </c>
-      <c r="H92" s="10">
-        <v>25</v>
-      </c>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
       <c r="I92" s="10">
         <f t="shared" si="5"/>
-        <v>26.5</v>
+        <v>0</v>
       </c>
       <c r="J92" s="10"/>
       <c r="K92" s="10"/>
@@ -4762,27 +4262,15 @@
       <c r="B93" s="10">
         <v>42</v>
       </c>
-      <c r="C93" s="10">
-        <v>0</v>
-      </c>
-      <c r="D93" s="10">
-        <v>0</v>
-      </c>
-      <c r="E93" s="10">
-        <v>0</v>
-      </c>
-      <c r="F93" s="10">
-        <v>0</v>
-      </c>
-      <c r="G93" s="10">
-        <v>28</v>
-      </c>
-      <c r="H93" s="10">
-        <v>26</v>
-      </c>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
       <c r="I93" s="10">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
@@ -4804,27 +4292,15 @@
       <c r="B94" s="10">
         <v>40</v>
       </c>
-      <c r="C94" s="10">
-        <v>0</v>
-      </c>
-      <c r="D94" s="10">
-        <v>0</v>
-      </c>
-      <c r="E94" s="10">
-        <v>0</v>
-      </c>
-      <c r="F94" s="10">
-        <v>0</v>
-      </c>
-      <c r="G94" s="10">
-        <v>26</v>
-      </c>
-      <c r="H94" s="10">
-        <v>26</v>
-      </c>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
       <c r="I94" s="10">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -4846,27 +4322,15 @@
       <c r="B95" s="10">
         <v>38</v>
       </c>
-      <c r="C95" s="10">
-        <v>0</v>
-      </c>
-      <c r="D95" s="10">
-        <v>0</v>
-      </c>
-      <c r="E95" s="10">
-        <v>0</v>
-      </c>
-      <c r="F95" s="10">
-        <v>0</v>
-      </c>
-      <c r="G95" s="10">
-        <v>25</v>
-      </c>
-      <c r="H95" s="10">
-        <v>26</v>
-      </c>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
       <c r="I95" s="10">
         <f t="shared" si="5"/>
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="J95" s="10"/>
       <c r="K95" s="10"/>
@@ -4888,27 +4352,15 @@
       <c r="B96" s="10">
         <v>35</v>
       </c>
-      <c r="C96" s="10">
-        <v>0</v>
-      </c>
-      <c r="D96" s="10">
-        <v>0</v>
-      </c>
-      <c r="E96" s="10">
-        <v>0</v>
-      </c>
-      <c r="F96" s="10">
-        <v>0</v>
-      </c>
-      <c r="G96" s="10">
-        <v>24</v>
-      </c>
-      <c r="H96" s="10">
-        <v>25</v>
-      </c>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
       <c r="I96" s="10">
         <f t="shared" si="5"/>
-        <v>24.5</v>
+        <v>0</v>
       </c>
       <c r="J96" s="10"/>
       <c r="K96" s="10"/>
@@ -4930,27 +4382,15 @@
       <c r="B97" s="10">
         <v>32</v>
       </c>
-      <c r="C97" s="10">
-        <v>0</v>
-      </c>
-      <c r="D97" s="10">
-        <v>0</v>
-      </c>
-      <c r="E97" s="10">
-        <v>0</v>
-      </c>
-      <c r="F97" s="10">
-        <v>0</v>
-      </c>
-      <c r="G97" s="10">
-        <v>23</v>
-      </c>
-      <c r="H97" s="10">
-        <v>24</v>
-      </c>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
       <c r="I97" s="10">
         <f t="shared" si="5"/>
-        <v>23.5</v>
+        <v>0</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -4972,27 +4412,15 @@
       <c r="B98" s="10">
         <v>30</v>
       </c>
-      <c r="C98" s="10">
-        <v>0</v>
-      </c>
-      <c r="D98" s="10">
-        <v>0</v>
-      </c>
-      <c r="E98" s="10">
-        <v>0</v>
-      </c>
-      <c r="F98" s="10">
-        <v>0</v>
-      </c>
-      <c r="G98" s="10">
-        <v>23</v>
-      </c>
-      <c r="H98" s="10">
-        <v>20</v>
-      </c>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
       <c r="I98" s="10">
         <f t="shared" si="5"/>
-        <v>21.5</v>
+        <v>0</v>
       </c>
       <c r="J98" s="10"/>
       <c r="K98" s="10"/>
@@ -5014,27 +4442,15 @@
       <c r="B99" s="10">
         <v>28</v>
       </c>
-      <c r="C99" s="10">
-        <v>0</v>
-      </c>
-      <c r="D99" s="10">
-        <v>0</v>
-      </c>
-      <c r="E99" s="10">
-        <v>0</v>
-      </c>
-      <c r="F99" s="10">
-        <v>0</v>
-      </c>
-      <c r="G99" s="10">
-        <v>19</v>
-      </c>
-      <c r="H99" s="10">
-        <v>23</v>
-      </c>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
       <c r="I99" s="10">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="J99" s="10"/>
       <c r="K99" s="10"/>
@@ -5056,27 +4472,15 @@
       <c r="B100" s="10">
         <v>25</v>
       </c>
-      <c r="C100" s="10">
-        <v>0</v>
-      </c>
-      <c r="D100" s="10">
-        <v>0</v>
-      </c>
-      <c r="E100" s="10">
-        <v>0</v>
-      </c>
-      <c r="F100" s="10">
-        <v>0</v>
-      </c>
-      <c r="G100" s="10">
-        <v>21</v>
-      </c>
-      <c r="H100" s="10">
-        <v>21</v>
-      </c>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
       <c r="I100" s="10">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -5398,24 +4802,12 @@
       <c r="B111" s="11">
         <v>25</v>
       </c>
-      <c r="C111" s="11">
-        <v>0</v>
-      </c>
-      <c r="D111" s="11">
-        <v>0</v>
-      </c>
-      <c r="E111" s="11">
-        <v>0</v>
-      </c>
-      <c r="F111" s="11">
-        <v>0</v>
-      </c>
-      <c r="G111" s="11">
-        <v>0</v>
-      </c>
-      <c r="H111" s="11">
-        <v>0</v>
-      </c>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11"/>
+      <c r="G111" s="11"/>
+      <c r="H111" s="11"/>
       <c r="I111" s="11">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5440,23 +4832,15 @@
       <c r="B112" s="2">
         <v>50</v>
       </c>
-      <c r="C112" s="2">
-        <v>1.452161</v>
-      </c>
+      <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
-      <c r="F112" s="2">
-        <v>355</v>
-      </c>
-      <c r="G112" s="2">
-        <v>439</v>
-      </c>
-      <c r="H112" s="2">
-        <v>408</v>
-      </c>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
       <c r="I112" s="2">
         <f t="shared" si="5"/>
-        <v>423.5</v>
+        <v>0</v>
       </c>
       <c r="J112" s="2">
         <v>0</v>
@@ -5478,23 +4862,15 @@
       <c r="B113" s="2">
         <v>48</v>
       </c>
-      <c r="C113" s="2">
-        <v>1.410256</v>
-      </c>
+      <c r="C113" s="2"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
-      <c r="F113" s="2">
-        <v>355</v>
-      </c>
-      <c r="G113" s="2">
-        <v>409</v>
-      </c>
-      <c r="H113" s="2">
-        <v>414</v>
-      </c>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
       <c r="I113" s="2">
         <f t="shared" si="5"/>
-        <v>411.5</v>
+        <v>0</v>
       </c>
       <c r="J113" s="2">
         <v>0</v>
@@ -5516,23 +4892,15 @@
       <c r="B114" s="2">
         <v>45</v>
       </c>
-      <c r="C114" s="2">
-        <v>1.349817</v>
-      </c>
+      <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
-      <c r="F114" s="2">
-        <v>354</v>
-      </c>
-      <c r="G114" s="2">
-        <v>393</v>
-      </c>
-      <c r="H114" s="2">
-        <v>386</v>
-      </c>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
       <c r="I114" s="2">
         <f t="shared" si="5"/>
-        <v>389.5</v>
+        <v>0</v>
       </c>
       <c r="J114" s="2">
         <v>0</v>
@@ -5554,23 +4922,15 @@
       <c r="B115" s="2">
         <v>42</v>
       </c>
-      <c r="C115" s="2">
-        <v>1.293407</v>
-      </c>
+      <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
-      <c r="F115" s="2">
-        <v>354</v>
-      </c>
-      <c r="G115" s="2">
-        <v>379</v>
-      </c>
-      <c r="H115" s="2">
-        <v>384</v>
-      </c>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
       <c r="I115" s="2">
         <f t="shared" si="5"/>
-        <v>381.5</v>
+        <v>0</v>
       </c>
       <c r="J115" s="2">
         <v>0</v>
@@ -5592,23 +4952,15 @@
       <c r="B116" s="2">
         <v>40</v>
       </c>
-      <c r="C116" s="2">
-        <v>1.2369300000000001</v>
-      </c>
+      <c r="C116" s="2"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
-      <c r="F116" s="2">
-        <v>350</v>
-      </c>
-      <c r="G116" s="2">
-        <v>387</v>
-      </c>
-      <c r="H116" s="2">
-        <v>363</v>
-      </c>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
       <c r="I116" s="2">
         <f t="shared" si="5"/>
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="J116" s="2">
         <v>0</v>
@@ -5630,23 +4982,15 @@
       <c r="B117" s="2">
         <v>38</v>
       </c>
-      <c r="C117" s="2">
-        <v>1.2023440000000001</v>
-      </c>
+      <c r="C117" s="2"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
-      <c r="F117" s="2">
-        <v>351</v>
-      </c>
-      <c r="G117" s="2">
-        <v>395</v>
-      </c>
-      <c r="H117" s="2">
-        <v>357</v>
-      </c>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
       <c r="I117" s="2">
         <f t="shared" si="5"/>
-        <v>376</v>
+        <v>0</v>
       </c>
       <c r="J117" s="2">
         <v>0</v>
@@ -5668,23 +5012,15 @@
       <c r="B118" s="2">
         <v>35</v>
       </c>
-      <c r="C118" s="2">
-        <v>1.1394869999999999</v>
-      </c>
+      <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
-      <c r="F118" s="2">
-        <v>349</v>
-      </c>
-      <c r="G118" s="2">
-        <v>385</v>
-      </c>
-      <c r="H118" s="2">
-        <v>337</v>
-      </c>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
       <c r="I118" s="2">
         <f t="shared" si="5"/>
-        <v>361</v>
+        <v>0</v>
       </c>
       <c r="J118" s="2">
         <v>0</v>
@@ -5706,23 +5042,15 @@
       <c r="B119" s="2">
         <v>32</v>
       </c>
-      <c r="C119" s="2">
-        <v>1.070989</v>
-      </c>
+      <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
-      <c r="F119" s="2">
-        <v>345</v>
-      </c>
-      <c r="G119" s="2">
-        <v>382</v>
-      </c>
-      <c r="H119" s="2">
-        <v>333</v>
-      </c>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
       <c r="I119" s="2">
         <f t="shared" si="5"/>
-        <v>357.5</v>
+        <v>0</v>
       </c>
       <c r="J119" s="2">
         <v>0</v>
@@ -5744,23 +5072,15 @@
       <c r="B120" s="2">
         <v>30</v>
       </c>
-      <c r="C120" s="2">
-        <v>1.033919</v>
-      </c>
+      <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
-      <c r="F120" s="2">
-        <v>345</v>
-      </c>
-      <c r="G120" s="2">
-        <v>324</v>
-      </c>
-      <c r="H120" s="2">
-        <v>376</v>
-      </c>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
       <c r="I120" s="2">
         <f t="shared" si="5"/>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="J120" s="2">
         <v>0</v>
@@ -5782,23 +5102,15 @@
       <c r="B121" s="2">
         <v>28</v>
       </c>
-      <c r="C121" s="2">
-        <v>0.99201499999999998</v>
-      </c>
+      <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
-      <c r="F121" s="2">
-        <v>344</v>
-      </c>
-      <c r="G121" s="2">
-        <v>311</v>
-      </c>
-      <c r="H121" s="2">
-        <v>372</v>
-      </c>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
       <c r="I121" s="2">
         <f t="shared" si="5"/>
-        <v>341.5</v>
+        <v>0</v>
       </c>
       <c r="J121" s="2">
         <v>0</v>
@@ -5820,23 +5132,15 @@
       <c r="B122" s="2">
         <v>25</v>
       </c>
-      <c r="C122" s="2">
-        <v>0.93640999999999996</v>
-      </c>
+      <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
-      <c r="F122" s="2">
-        <v>344</v>
-      </c>
-      <c r="G122" s="2">
-        <v>362</v>
-      </c>
-      <c r="H122" s="2">
-        <v>302</v>
-      </c>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
       <c r="I122" s="2">
         <f t="shared" si="5"/>
-        <v>332</v>
+        <v>0</v>
       </c>
       <c r="J122" s="2">
         <v>0</v>
@@ -13093,12 +12397,10 @@
       <c r="E364" s="17"/>
       <c r="F364" s="17"/>
       <c r="G364" s="17"/>
-      <c r="H364" s="17">
-        <v>12</v>
-      </c>
+      <c r="H364" s="17"/>
       <c r="I364" s="17">
-        <f>(H364+G364)/2</f>
-        <v>6</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="J364" s="17">
         <v>3</v>

</xml_diff>